<commit_message>
Added exhaust temperature capability to HW and SW
</commit_message>
<xml_diff>
--- a/hw/bom.xlsx
+++ b/hw/bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25217"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25906"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1a1d\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{5EED3EE9-8CBF-46A4-B322-1A61DCFFCBFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99EFC6EA-AD7F-4001-A4EC-5D646D5003FA}"/>
+  <xr:revisionPtr revIDLastSave="192" documentId="8_{5EED3EE9-8CBF-46A4-B322-1A61DCFFCBFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{654A0B0D-9882-4772-9D9E-A0727C5D6826}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,6 +25,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="126">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -124,7 +125,7 @@
     <t>MAL203855221E3</t>
   </si>
   <si>
-    <t>220uf electrolytic capacitor 15V</t>
+    <t>220uf electrolytic capacitor 10V</t>
   </si>
   <si>
     <t>684-1914</t>
@@ -398,6 +399,15 @@
   </si>
   <si>
     <t>LED holder 5mm</t>
+  </si>
+  <si>
+    <t>Resistor 9K31 0.1%</t>
+  </si>
+  <si>
+    <t>754-7095</t>
+  </si>
+  <si>
+    <t>R7, R10</t>
   </si>
   <si>
     <t>Total</t>
@@ -805,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -886,7 +896,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -899,7 +909,7 @@
       </c>
       <c r="H3" s="1">
         <f>D3*G3</f>
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>17</v>
@@ -928,7 +938,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>19</v>
@@ -1663,13 +1673,36 @@
         <v>22</v>
       </c>
     </row>
+    <row r="35" spans="1:9">
+      <c r="C35" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G35" s="1">
+        <v>64</v>
+      </c>
+      <c r="H35" s="1">
+        <v>128</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
     <row r="36" spans="1:9">
       <c r="F36" s="4" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H36" s="1">
-        <f>SUM(H2:H34)</f>
-        <v>4762</v>
+        <f>SUM(H2:H35)</f>
+        <v>4906</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates for hardware version 2.0
</commit_message>
<xml_diff>
--- a/hw/bom.xlsx
+++ b/hw/bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25906"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1a1d\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="192" documentId="8_{5EED3EE9-8CBF-46A4-B322-1A61DCFFCBFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{654A0B0D-9882-4772-9D9E-A0727C5D6826}"/>
+  <xr:revisionPtr revIDLastSave="193" documentId="8_{5EED3EE9-8CBF-46A4-B322-1A61DCFFCBFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97BC066C-49C5-4316-88D5-0CDFD1E270E7}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,7 +98,7 @@
     <t>100nf ceramic capacitor</t>
   </si>
   <si>
-    <t>C2</t>
+    <t>C2, C6, C7</t>
   </si>
   <si>
     <t>Nichicon</t>
@@ -815,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>

</xml_diff>